<commit_message>
added error emails handling
</commit_message>
<xml_diff>
--- a/uploads/TrySheet2.xlsx
+++ b/uploads/TrySheet2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9144"/>
+    <workbookView windowWidth="23040" windowHeight="8700"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,9 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>anshumanpandey182005@gmail.com</t>
+  </si>
+  <si>
+    <t>panda182005@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -53,18 +56,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -499,28 +502,28 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -644,10 +647,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1126,7 +1130,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6296296296296" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -1142,12 +1146,15 @@
       <c r="B1" s="2"/>
     </row>
     <row r="2" customHeight="1" spans="1:2">
-      <c r="A2" s="2"/>
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
       <c r="B2" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" display="anshumanpandey182005@gmail.com"/>
+    <hyperlink ref="A2" r:id="rId2" display="panda182005@gmail.com" tooltip="mailto:panda182005@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>